<commit_message>
implementing new seeds for Medias
</commit_message>
<xml_diff>
--- a/src/integrator/files/kondos.xlsx
+++ b/src/integrator/files/kondos.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="289">
   <si>
     <t>slug</t>
   </si>
@@ -672,6 +672,15 @@
     <t>Serra Morena</t>
   </si>
   <si>
+    <t>to-upload</t>
+  </si>
+  <si>
+    <t>O condomínio Serra Morena tem um perfil rústico, com muito contato com a natureza e atividades ao ar livre.
+O charme de roça aumenta com a igrejinha e os patos que ficam em volta da lagoa.
+Conta também com quadras, campo de futebol, um restaurante e até uma academia.
+Para os amantes de natureza e da natureza, é um bom custo benefício e uma excelente escolha.</t>
+  </si>
+  <si>
     <t>Fazendinhas Eldorado</t>
   </si>
   <si>
@@ -741,13 +750,13 @@
     <t>Balneário Vista da Lagoa</t>
   </si>
   <si>
+    <t>archived</t>
+  </si>
+  <si>
     <t>Com natureza exuberante, o condomínio fornece lotes com escritura, registro e financiamento próprio.</t>
   </si>
   <si>
     <t>La Ville</t>
-  </si>
-  <si>
-    <t>media-gathering</t>
   </si>
   <si>
     <t>La Ville é um condomínio fechado com venda de casas prontas.
@@ -776,10 +785,23 @@
     <t>Fazendas Terras de Minas</t>
   </si>
   <si>
+    <t>Localizada em Piedade do Paraopeba, um povoado com mais de 300 anos de história, no sopé da Serra da Moeda, o condomínio Fazendas Terras de Minas carrega toda a cultura e o significado do que é ser mineiro. 
+Conectado com a paz da natureza, você vai ficar perto das casas coloniais, de igrejas centenárias, fazendas, alambiques, mirantes, casas de artesanato, pousadas e restaurantes com os mais tradicionais sabores da cozinha mineira.
+O condomínio é completo, e conta com conveniências de um ótimo padrão.
+• Infraestrutura completa para viver com conforto, lazer e segurança;
+• Áreas com potencial produtivo e rica variedade de fauna e flora nativa;
+• Arquitetura que une design ao charme da vida no campo;
+• A apenas 40 minutos do BH Shopping, com duas opções de rotas de acesso
+ pela BR-040.</t>
+  </si>
+  <si>
     <t>Piedade do Paraopeba</t>
   </si>
   <si>
     <t>Vila Castela Brisas</t>
+  </si>
+  <si>
+    <t>media-gathering</t>
   </si>
   <si>
     <t>Vila Castela é um conjunto de 9 condomínios de alto padrão, localizado na região de Nova Lima, bem próximo ao Vila da Serra.
@@ -809,6 +831,84 @@
   </si>
   <si>
     <t>Vila Castela Reserva</t>
+  </si>
+  <si>
+    <t>Alto dos Pinheiros</t>
+  </si>
+  <si>
+    <t>Uma pérola de condomínio, com a mais alta modernidade e um toque de sofisticação, o Alto dos Pinheiros é um condomínio premium.
+O Alto dos Pinheiros conta com lazer de primeira e uma variedade de recursos de entretenimento e segurança que atendem até os mais exigentes.
+Com completo suporte para esportes, tendo quadras de tênis, beach tennis, também provém de muitas opções para recreação de todas as idades.</t>
+  </si>
+  <si>
+    <t>Capim Branco</t>
+  </si>
+  <si>
+    <t>Mãe Terra</t>
+  </si>
+  <si>
+    <t>Um refúgio perfeito localizado na encantadora encosta da Serra da Moeda, no vale do Paraopeba em Brumadinho. Este condomínio se destaca por sua localização privilegiada em uma área de imensa beleza natural e tranquilidade, oferecendo um ambiente ideal para aqueles que desejam escapar do caos urbano e se reconectar com a natureza.
+Os lotes no Condomínio Mãe Terra são parte de uma comunidade planejada com apenas 186 lotes, garantindo exclusividade e uma sensação de comunidade mais íntima e tranquila. A segurança é uma prioridade, com serviço de portaria 24 horas para garantir o bem-estar de todos os moradores.
+Os admiradores da natureza ficarão encantados com a rica fauna e flora que circundam o local, incluindo uma vasta área de preservação permanente que assegura a manutenção da beleza natural do ambiente. Essa riqueza ecológica proporciona um cenário deslumbrante e oportunidades únicas para observação de aves, caminhadas e outras atividades ao ar livre diretamente no seu quintal.
+O condomínio foi projetado com uma infraestrutura urbana de alta qualidade, com ruas pavimentadas com blocos intertravados que se integram harmoniosamente ao ambiente natural. Esse cuidado com a infraestrutura garante não só a durabilidade e a estética, mas também contribui para uma gestão sustentável das águas pluviais.
+Investir em um lote no Condomínio Mãe Terra é escolher um estilo de vida em harmonia com a natureza, sem abrir mão do conforto e da segurança. É o local ideal para construir a casa dos seus sonhos e desfrutar de uma qualidade de vida inigualável, onde cada dia é uma nova oportunidade para se sentir revitalizado e inspirado pela beleza natural do entorno.</t>
+  </si>
+  <si>
+    <t>Vale do Paraopeba</t>
+  </si>
+  <si>
+    <t>Aguas do Funil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	O condomínio náutico Águas do Funil fica na cidade de Perdões, MG, bem próximo de Lavras, a 3 horas de BH.
+	No formato de ilha, o condomínio é rodeado pelas águas da represa de Perdões.
+	Apesar de se auto-denominar de luxo, o condomínio conta com recursos de nível B, como espaço gourmet, quadras, playground e marina.
+	O condomínio é um ótimo custo-benefício para os amantes de atividades aquáticas junto à natureza.</t>
+  </si>
+  <si>
+    <t>ciclope empreendimentos</t>
+  </si>
+  <si>
+    <t>Perdões</t>
+  </si>
+  <si>
+    <t>Versailles</t>
+  </si>
+  <si>
+    <t>O Versailles está localizado em lagoa santa, fica ao lado do Condominio Eco Village á 10min da lagoa central.
+O condomínio, que conta com portaria 24h, quadras esportivas, piscinas e áreas verdes, já está sendo habitado por moradores.
+São lotes a partir de 1000m² com valor á partir de R$ 250.000,00, com financiamento próprio e lotes de revendas que podem ser financiados pelo banco.</t>
+  </si>
+  <si>
+    <t>match imob</t>
+  </si>
+  <si>
+    <t>Gândara</t>
+  </si>
+  <si>
+    <t>O surpreendente condomínio Gândara, situado próximo à Serra do Gandarela, fica no município de Rio Acima, um pouco depois de Nova Lima.
+O condomínio possui segurança 24 horas, área de convivência, lagoa e cachoeira privativa.
+Com uma grande área verde preservada, o condomínio surpreende com os diferenciais, e os valores, que estão saindo a partir de 890 mil, podem ser financiados em até 60x com a incorporadora.</t>
+  </si>
+  <si>
+    <t>Rio Acima</t>
+  </si>
+  <si>
+    <t>Estância da Lapa</t>
+  </si>
+  <si>
+    <t>Mocambeiro, uma região que sempre inspirou sonhos e planos,
+hoje é o cenário para você abraçar a liberdade e escrever
+o melhor capítulo da sua história. Para você se reconectar
+com suas origens e aproveitar tudo que a natureza oferece de
+melhor: bem-estar, boas energias e muitas alegrias.
+A apenas 45 minutos de BH, o Estância da Lapa pode te surpreender, com belo paisagismo, praças, e bons terrenos, de 20mil m², para se desenvolver uma fazendinha.</t>
+  </si>
+  <si>
+    <t>Balneário Shangrylá</t>
+  </si>
+  <si>
+    <t>Loteamento</t>
   </si>
   <si>
     <t>IDKONDO</t>
@@ -868,10 +968,10 @@
     <t>Prédios</t>
   </si>
   <si>
-    <t>done</t>
+    <t>Comercial</t>
   </si>
   <si>
-    <t>Comercial</t>
+    <t>done</t>
   </si>
   <si>
     <t>Industrial</t>
@@ -1610,7 +1710,8 @@
     <col customWidth="1" min="4" max="4" width="16.25"/>
     <col customWidth="1" min="5" max="5" width="14.88"/>
     <col customWidth="1" min="6" max="6" width="9.63"/>
-    <col customWidth="1" min="7" max="8" width="17.25"/>
+    <col customWidth="1" min="7" max="7" width="21.13"/>
+    <col customWidth="1" min="8" max="8" width="17.25"/>
     <col customWidth="1" min="9" max="9" width="12.25"/>
     <col customWidth="1" min="10" max="10" width="13.0"/>
     <col customWidth="1" min="11" max="11" width="21.88"/>
@@ -1643,7 +1744,7 @@
     <col customWidth="1" min="38" max="38" width="11.75"/>
     <col customWidth="1" min="39" max="39" width="21.63"/>
     <col customWidth="1" min="40" max="40" width="16.0"/>
-    <col customWidth="1" min="41" max="41" width="18.88"/>
+    <col customWidth="1" min="41" max="41" width="20.0"/>
     <col customWidth="1" min="42" max="42" width="13.5"/>
     <col customWidth="1" min="43" max="43" width="18.0"/>
     <col customWidth="1" min="44" max="44" width="16.25"/>
@@ -8046,7 +8147,9 @@
         <v>58</v>
       </c>
       <c r="E89" s="18"/>
-      <c r="F89" s="32"/>
+      <c r="F89" s="32" t="s">
+        <v>138</v>
+      </c>
       <c r="G89" s="30"/>
       <c r="H89" s="30">
         <v>280000.0</v>
@@ -8255,54 +8358,92 @@
         <v>57</v>
       </c>
       <c r="D92" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E92" s="31"/>
-      <c r="F92" s="19"/>
+        <v>211</v>
+      </c>
+      <c r="E92" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="F92" s="32" t="s">
+        <v>138</v>
+      </c>
       <c r="G92" s="20"/>
-      <c r="H92" s="20"/>
-      <c r="I92" s="22"/>
-      <c r="J92" s="22"/>
+      <c r="H92" s="30">
+        <v>170000.0</v>
+      </c>
+      <c r="I92" s="16">
+        <v>350.0</v>
+      </c>
+      <c r="J92" s="16">
+        <v>1.0</v>
+      </c>
       <c r="K92" s="21">
         <v>1000.0</v>
       </c>
-      <c r="L92" s="22"/>
+      <c r="L92" s="16">
+        <v>120.0</v>
+      </c>
       <c r="M92" s="22"/>
       <c r="N92" s="29"/>
       <c r="O92" s="16" t="s">
         <v>69</v>
       </c>
       <c r="P92" s="22"/>
-      <c r="Q92" s="22"/>
-      <c r="R92" s="22"/>
+      <c r="Q92" s="16">
+        <v>1.0</v>
+      </c>
+      <c r="R92" s="16">
+        <v>120.0</v>
+      </c>
       <c r="S92" s="22"/>
       <c r="T92" s="22"/>
       <c r="U92" s="24"/>
-      <c r="V92" s="25"/>
+      <c r="V92" s="34">
+        <v>1.0</v>
+      </c>
       <c r="W92" s="25"/>
-      <c r="X92" s="25"/>
-      <c r="Y92" s="25"/>
+      <c r="X92" s="34">
+        <v>1.0</v>
+      </c>
+      <c r="Y92" s="34">
+        <v>1.0</v>
+      </c>
       <c r="Z92" s="26"/>
       <c r="AA92" s="26"/>
-      <c r="AB92" s="26"/>
+      <c r="AB92" s="35"/>
       <c r="AC92" s="26"/>
       <c r="AD92" s="26"/>
-      <c r="AE92" s="26"/>
-      <c r="AF92" s="26"/>
-      <c r="AG92" s="26"/>
-      <c r="AH92" s="26"/>
+      <c r="AE92" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AF92" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG92" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH92" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AI92" s="26"/>
       <c r="AJ92" s="26"/>
-      <c r="AK92" s="26"/>
+      <c r="AK92" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AL92" s="26"/>
       <c r="AM92" s="26"/>
-      <c r="AN92" s="26"/>
+      <c r="AN92" s="35"/>
       <c r="AO92" s="26"/>
-      <c r="AP92" s="26"/>
-      <c r="AQ92" s="26"/>
+      <c r="AP92" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AQ92" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AR92" s="26"/>
       <c r="AS92" s="26"/>
-      <c r="AT92" s="26"/>
+      <c r="AT92" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AU92" s="26"/>
       <c r="AV92" s="26"/>
       <c r="AW92" s="26"/>
@@ -8317,7 +8458,7 @@
     <row r="93">
       <c r="A93" s="28"/>
       <c r="B93" s="15" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C93" s="16" t="s">
         <v>57</v>
@@ -8385,7 +8526,7 @@
     <row r="94">
       <c r="A94" s="28"/>
       <c r="B94" s="14" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C94" s="16" t="s">
         <v>57</v>
@@ -8408,7 +8549,7 @@
       <c r="M94" s="26"/>
       <c r="N94" s="42"/>
       <c r="O94" s="35" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="P94" s="26"/>
       <c r="Q94" s="26"/>
@@ -8416,7 +8557,7 @@
       <c r="S94" s="26"/>
       <c r="T94" s="26"/>
       <c r="U94" s="56" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="V94" s="55"/>
       <c r="W94" s="55"/>
@@ -8457,7 +8598,7 @@
     <row r="95">
       <c r="A95" s="28"/>
       <c r="B95" s="14" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C95" s="16" t="s">
         <v>57</v>
@@ -8480,7 +8621,7 @@
       <c r="M95" s="26"/>
       <c r="N95" s="42"/>
       <c r="O95" s="35" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="P95" s="26"/>
       <c r="Q95" s="26"/>
@@ -8488,7 +8629,7 @@
       <c r="S95" s="26"/>
       <c r="T95" s="26"/>
       <c r="U95" s="60" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="V95" s="61"/>
       <c r="W95" s="61"/>
@@ -8529,7 +8670,7 @@
     <row r="96">
       <c r="A96" s="28"/>
       <c r="B96" s="14" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C96" s="26"/>
       <c r="D96" s="17" t="s">
@@ -8593,7 +8734,7 @@
     <row r="97">
       <c r="A97" s="28"/>
       <c r="B97" s="14" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C97" s="35" t="s">
         <v>57</v>
@@ -8624,7 +8765,7 @@
       <c r="S97" s="26"/>
       <c r="T97" s="26"/>
       <c r="U97" s="60" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="V97" s="61">
         <v>1.0</v>
@@ -8682,7 +8823,7 @@
       <c r="AY97" s="26"/>
       <c r="AZ97" s="27"/>
       <c r="BA97" s="65" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="BB97" s="27"/>
       <c r="BC97" s="27"/>
@@ -8691,16 +8832,16 @@
     <row r="98">
       <c r="A98" s="28"/>
       <c r="B98" s="14" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C98" s="35" t="s">
         <v>82</v>
       </c>
       <c r="D98" s="17" t="s">
-        <v>58</v>
+        <v>225</v>
       </c>
       <c r="E98" s="17" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="F98" s="59"/>
       <c r="G98" s="21"/>
@@ -8761,22 +8902,22 @@
     <row r="99">
       <c r="A99" s="28"/>
       <c r="B99" s="14" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C99" s="35" t="s">
         <v>57</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="E99" s="17" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F99" s="59" t="s">
         <v>138</v>
       </c>
       <c r="G99" s="21" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H99" s="21"/>
       <c r="I99" s="35">
@@ -8789,13 +8930,13 @@
       </c>
       <c r="M99" s="26"/>
       <c r="N99" s="66" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="O99" s="35" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="P99" s="35" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="Q99" s="35">
         <v>1.0</v>
@@ -8863,20 +9004,24 @@
     <row r="100">
       <c r="A100" s="28"/>
       <c r="B100" s="14" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C100" s="35" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="E100" s="17"/>
+        <v>211</v>
+      </c>
+      <c r="E100" s="17" t="s">
+        <v>234</v>
+      </c>
       <c r="F100" s="59" t="s">
         <v>138</v>
       </c>
       <c r="G100" s="21"/>
-      <c r="H100" s="21"/>
+      <c r="H100" s="21">
+        <v>600000.0</v>
+      </c>
       <c r="I100" s="26"/>
       <c r="J100" s="35">
         <v>1.0</v>
@@ -8884,14 +9029,18 @@
       <c r="K100" s="21">
         <v>20000.0</v>
       </c>
-      <c r="L100" s="26"/>
+      <c r="L100" s="35">
+        <v>40.0</v>
+      </c>
       <c r="M100" s="26"/>
       <c r="N100" s="27"/>
       <c r="O100" s="35" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="P100" s="26"/>
-      <c r="Q100" s="26"/>
+      <c r="Q100" s="35">
+        <v>1.0</v>
+      </c>
       <c r="R100" s="26"/>
       <c r="S100" s="26"/>
       <c r="T100" s="26"/>
@@ -8977,16 +9126,16 @@
     <row r="101">
       <c r="A101" s="28"/>
       <c r="B101" s="15" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C101" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="E101" s="18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F101" s="32" t="s">
         <v>138</v>
@@ -9077,16 +9226,16 @@
     <row r="102">
       <c r="A102" s="28"/>
       <c r="B102" s="14" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="C102" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="E102" s="18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F102" s="59" t="s">
         <v>138</v>
@@ -9177,16 +9326,16 @@
     <row r="103">
       <c r="A103" s="28"/>
       <c r="B103" s="14" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C103" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="E103" s="18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F103" s="59" t="s">
         <v>138</v>
@@ -9277,16 +9426,16 @@
     <row r="104">
       <c r="A104" s="28"/>
       <c r="B104" s="14" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C104" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="E104" s="18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F104" s="59" t="s">
         <v>138</v>
@@ -9377,16 +9526,16 @@
     <row r="105">
       <c r="A105" s="28"/>
       <c r="B105" s="14" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="C105" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="E105" s="18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F105" s="59" t="s">
         <v>138</v>
@@ -9477,16 +9626,16 @@
     <row r="106">
       <c r="A106" s="28"/>
       <c r="B106" s="14" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C106" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="E106" s="18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F106" s="59" t="s">
         <v>138</v>
@@ -9577,16 +9726,16 @@
     <row r="107">
       <c r="A107" s="28"/>
       <c r="B107" s="14" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C107" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="E107" s="18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F107" s="59" t="s">
         <v>138</v>
@@ -9683,16 +9832,16 @@
     <row r="108">
       <c r="A108" s="28"/>
       <c r="B108" s="14" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C108" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="E108" s="18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F108" s="59" t="s">
         <v>138</v>
@@ -9783,16 +9932,16 @@
     <row r="109">
       <c r="A109" s="28"/>
       <c r="B109" s="14" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C109" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D109" s="18" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="E109" s="18" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="F109" s="59" t="s">
         <v>138</v>
@@ -9892,54 +10041,114 @@
     </row>
     <row r="110">
       <c r="A110" s="28"/>
-      <c r="B110" s="14"/>
-      <c r="C110" s="26"/>
-      <c r="D110" s="17"/>
-      <c r="E110" s="17"/>
-      <c r="F110" s="59"/>
+      <c r="B110" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C110" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D110" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E110" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="F110" s="59" t="s">
+        <v>138</v>
+      </c>
       <c r="G110" s="21"/>
-      <c r="H110" s="21"/>
-      <c r="I110" s="26"/>
-      <c r="J110" s="26"/>
-      <c r="K110" s="63"/>
-      <c r="L110" s="26"/>
+      <c r="H110" s="21">
+        <v>150000.0</v>
+      </c>
+      <c r="I110" s="35">
+        <v>400.0</v>
+      </c>
+      <c r="J110" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="K110" s="21">
+        <v>360.0</v>
+      </c>
+      <c r="L110" s="35">
+        <v>50.0</v>
+      </c>
       <c r="M110" s="26"/>
       <c r="N110" s="27"/>
-      <c r="O110" s="26"/>
+      <c r="O110" s="35" t="s">
+        <v>249</v>
+      </c>
       <c r="P110" s="26"/>
-      <c r="Q110" s="26"/>
-      <c r="R110" s="26"/>
+      <c r="Q110" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="R110" s="35">
+        <v>48.0</v>
+      </c>
       <c r="S110" s="26"/>
       <c r="T110" s="26"/>
       <c r="U110" s="64"/>
-      <c r="V110" s="55"/>
-      <c r="W110" s="55"/>
-      <c r="X110" s="55"/>
-      <c r="Y110" s="55"/>
-      <c r="Z110" s="26"/>
-      <c r="AA110" s="26"/>
-      <c r="AB110" s="26"/>
+      <c r="V110" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="W110" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="X110" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="Y110" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="Z110" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AA110" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AB110" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AC110" s="26"/>
-      <c r="AD110" s="26"/>
+      <c r="AD110" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AE110" s="26"/>
-      <c r="AF110" s="26"/>
-      <c r="AG110" s="26"/>
-      <c r="AH110" s="26"/>
-      <c r="AI110" s="26"/>
+      <c r="AF110" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG110" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH110" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AI110" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AJ110" s="26"/>
-      <c r="AK110" s="26"/>
+      <c r="AK110" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AL110" s="26"/>
       <c r="AM110" s="26"/>
       <c r="AN110" s="26"/>
       <c r="AO110" s="26"/>
-      <c r="AP110" s="26"/>
-      <c r="AQ110" s="26"/>
+      <c r="AP110" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AQ110" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AR110" s="26"/>
       <c r="AS110" s="26"/>
-      <c r="AT110" s="26"/>
+      <c r="AT110" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AU110" s="26"/>
       <c r="AV110" s="26"/>
-      <c r="AW110" s="26"/>
+      <c r="AW110" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AX110" s="26"/>
       <c r="AY110" s="26"/>
       <c r="AZ110" s="27"/>
@@ -9950,29 +10159,57 @@
     </row>
     <row r="111">
       <c r="A111" s="28"/>
-      <c r="B111" s="14"/>
-      <c r="C111" s="26"/>
-      <c r="D111" s="17"/>
-      <c r="E111" s="17"/>
-      <c r="F111" s="59"/>
+      <c r="B111" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="C111" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D111" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E111" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="F111" s="59" t="s">
+        <v>138</v>
+      </c>
       <c r="G111" s="21"/>
-      <c r="H111" s="21"/>
-      <c r="I111" s="26"/>
-      <c r="J111" s="26"/>
-      <c r="K111" s="63"/>
-      <c r="L111" s="26"/>
+      <c r="H111" s="21">
+        <v>160000.0</v>
+      </c>
+      <c r="I111" s="35">
+        <v>240.0</v>
+      </c>
+      <c r="J111" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="K111" s="21">
+        <v>1010.0</v>
+      </c>
+      <c r="L111" s="35">
+        <v>35.0</v>
+      </c>
       <c r="M111" s="26"/>
       <c r="N111" s="27"/>
-      <c r="O111" s="26"/>
-      <c r="P111" s="26"/>
+      <c r="O111" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="P111" s="35" t="s">
+        <v>252</v>
+      </c>
       <c r="Q111" s="26"/>
       <c r="R111" s="26"/>
       <c r="S111" s="26"/>
       <c r="T111" s="26"/>
       <c r="U111" s="64"/>
-      <c r="V111" s="55"/>
+      <c r="V111" s="61">
+        <v>1.0</v>
+      </c>
       <c r="W111" s="55"/>
-      <c r="X111" s="55"/>
+      <c r="X111" s="61">
+        <v>1.0</v>
+      </c>
       <c r="Y111" s="55"/>
       <c r="Z111" s="26"/>
       <c r="AA111" s="26"/>
@@ -9980,17 +10217,25 @@
       <c r="AC111" s="26"/>
       <c r="AD111" s="26"/>
       <c r="AE111" s="26"/>
-      <c r="AF111" s="26"/>
-      <c r="AG111" s="26"/>
-      <c r="AH111" s="26"/>
+      <c r="AF111" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG111" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH111" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AI111" s="26"/>
       <c r="AJ111" s="26"/>
-      <c r="AK111" s="26"/>
-      <c r="AL111" s="26"/>
+      <c r="AK111" s="35"/>
+      <c r="AL111" s="35"/>
       <c r="AM111" s="26"/>
       <c r="AN111" s="26"/>
       <c r="AO111" s="26"/>
-      <c r="AP111" s="26"/>
+      <c r="AP111" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AQ111" s="26"/>
       <c r="AR111" s="26"/>
       <c r="AS111" s="26"/>
@@ -10008,48 +10253,98 @@
     </row>
     <row r="112">
       <c r="A112" s="28"/>
-      <c r="B112" s="14"/>
-      <c r="C112" s="26"/>
-      <c r="D112" s="17"/>
-      <c r="E112" s="17"/>
-      <c r="F112" s="59"/>
-      <c r="G112" s="21"/>
-      <c r="H112" s="21"/>
-      <c r="I112" s="26"/>
-      <c r="J112" s="26"/>
-      <c r="K112" s="63"/>
-      <c r="L112" s="26"/>
+      <c r="B112" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C112" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D112" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E112" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="F112" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="G112" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="H112" s="21">
+        <v>160000.0</v>
+      </c>
+      <c r="I112" s="35">
+        <v>200.0</v>
+      </c>
+      <c r="J112" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="K112" s="21">
+        <v>636.0</v>
+      </c>
+      <c r="L112" s="35">
+        <v>180.0</v>
+      </c>
       <c r="M112" s="26"/>
       <c r="N112" s="27"/>
-      <c r="O112" s="26"/>
+      <c r="O112" s="35" t="s">
+        <v>256</v>
+      </c>
       <c r="P112" s="26"/>
-      <c r="Q112" s="26"/>
-      <c r="R112" s="26"/>
+      <c r="Q112" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="R112" s="35">
+        <v>60.0</v>
+      </c>
       <c r="S112" s="26"/>
       <c r="T112" s="26"/>
       <c r="U112" s="64"/>
-      <c r="V112" s="55"/>
+      <c r="V112" s="61">
+        <v>1.0</v>
+      </c>
       <c r="W112" s="55"/>
-      <c r="X112" s="55"/>
-      <c r="Y112" s="55"/>
+      <c r="X112" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="Y112" s="61">
+        <v>1.0</v>
+      </c>
       <c r="Z112" s="26"/>
       <c r="AA112" s="26"/>
-      <c r="AB112" s="26"/>
+      <c r="AB112" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AC112" s="26"/>
-      <c r="AD112" s="26"/>
-      <c r="AE112" s="26"/>
-      <c r="AF112" s="26"/>
-      <c r="AG112" s="26"/>
-      <c r="AH112" s="26"/>
+      <c r="AD112" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AE112" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AF112" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG112" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH112" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AI112" s="26"/>
       <c r="AJ112" s="26"/>
-      <c r="AK112" s="26"/>
+      <c r="AK112" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AL112" s="26"/>
       <c r="AM112" s="26"/>
       <c r="AN112" s="26"/>
       <c r="AO112" s="26"/>
       <c r="AP112" s="26"/>
-      <c r="AQ112" s="26"/>
+      <c r="AQ112" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AR112" s="26"/>
       <c r="AS112" s="26"/>
       <c r="AT112" s="26"/>
@@ -10066,39 +10361,79 @@
     </row>
     <row r="113">
       <c r="A113" s="28"/>
-      <c r="B113" s="14"/>
-      <c r="C113" s="26"/>
-      <c r="D113" s="17"/>
-      <c r="E113" s="17"/>
-      <c r="F113" s="59"/>
-      <c r="G113" s="21"/>
-      <c r="H113" s="21"/>
-      <c r="I113" s="26"/>
-      <c r="J113" s="26"/>
-      <c r="K113" s="63"/>
-      <c r="L113" s="26"/>
+      <c r="B113" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C113" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D113" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E113" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="F113" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="G113" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="H113" s="21">
+        <v>250000.0</v>
+      </c>
+      <c r="I113" s="35">
+        <v>400.0</v>
+      </c>
+      <c r="J113" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="K113" s="21">
+        <v>1000.0</v>
+      </c>
+      <c r="L113" s="35">
+        <v>50.0</v>
+      </c>
       <c r="M113" s="26"/>
       <c r="N113" s="27"/>
-      <c r="O113" s="26"/>
+      <c r="O113" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="P113" s="26"/>
-      <c r="Q113" s="26"/>
+      <c r="Q113" s="35">
+        <v>1.0</v>
+      </c>
       <c r="R113" s="26"/>
       <c r="S113" s="26"/>
       <c r="T113" s="26"/>
       <c r="U113" s="64"/>
-      <c r="V113" s="55"/>
+      <c r="V113" s="61">
+        <v>1.0</v>
+      </c>
       <c r="W113" s="55"/>
-      <c r="X113" s="55"/>
-      <c r="Y113" s="55"/>
+      <c r="X113" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="Y113" s="61">
+        <v>1.0</v>
+      </c>
       <c r="Z113" s="26"/>
-      <c r="AA113" s="26"/>
+      <c r="AA113" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AB113" s="26"/>
       <c r="AC113" s="26"/>
       <c r="AD113" s="26"/>
       <c r="AE113" s="26"/>
-      <c r="AF113" s="26"/>
-      <c r="AG113" s="26"/>
-      <c r="AH113" s="26"/>
+      <c r="AF113" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG113" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH113" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AI113" s="26"/>
       <c r="AJ113" s="26"/>
       <c r="AK113" s="26"/>
@@ -10107,7 +10442,9 @@
       <c r="AN113" s="26"/>
       <c r="AO113" s="26"/>
       <c r="AP113" s="26"/>
-      <c r="AQ113" s="26"/>
+      <c r="AQ113" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AR113" s="26"/>
       <c r="AS113" s="26"/>
       <c r="AT113" s="26"/>
@@ -10115,7 +10452,7 @@
       <c r="AV113" s="26"/>
       <c r="AW113" s="26"/>
       <c r="AX113" s="26"/>
-      <c r="AY113" s="26"/>
+      <c r="AY113" s="35"/>
       <c r="AZ113" s="27"/>
       <c r="BA113" s="27"/>
       <c r="BB113" s="27"/>
@@ -10124,47 +10461,95 @@
     </row>
     <row r="114">
       <c r="A114" s="28"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="26"/>
-      <c r="D114" s="17"/>
-      <c r="E114" s="17"/>
-      <c r="F114" s="59"/>
+      <c r="B114" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C114" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D114" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E114" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="F114" s="59" t="s">
+        <v>138</v>
+      </c>
       <c r="G114" s="21"/>
-      <c r="H114" s="21"/>
+      <c r="H114" s="21">
+        <v>900000.0</v>
+      </c>
       <c r="I114" s="26"/>
-      <c r="J114" s="26"/>
-      <c r="K114" s="63"/>
-      <c r="L114" s="26"/>
+      <c r="J114" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="K114" s="21">
+        <v>20000.0</v>
+      </c>
+      <c r="L114" s="35">
+        <v>55.0</v>
+      </c>
       <c r="M114" s="26"/>
       <c r="N114" s="27"/>
-      <c r="O114" s="26"/>
+      <c r="O114" s="35" t="s">
+        <v>262</v>
+      </c>
       <c r="P114" s="26"/>
-      <c r="Q114" s="26"/>
-      <c r="R114" s="26"/>
+      <c r="Q114" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="R114" s="35">
+        <v>60.0</v>
+      </c>
       <c r="S114" s="26"/>
       <c r="T114" s="26"/>
       <c r="U114" s="64"/>
-      <c r="V114" s="55"/>
-      <c r="W114" s="55"/>
-      <c r="X114" s="55"/>
+      <c r="V114" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="W114" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="X114" s="61">
+        <v>1.0</v>
+      </c>
       <c r="Y114" s="55"/>
       <c r="Z114" s="26"/>
       <c r="AA114" s="26"/>
       <c r="AB114" s="26"/>
       <c r="AC114" s="26"/>
       <c r="AD114" s="26"/>
-      <c r="AE114" s="26"/>
-      <c r="AF114" s="26"/>
-      <c r="AG114" s="26"/>
-      <c r="AH114" s="26"/>
-      <c r="AI114" s="26"/>
+      <c r="AE114" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AF114" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG114" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH114" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AI114" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AJ114" s="26"/>
-      <c r="AK114" s="26"/>
-      <c r="AL114" s="26"/>
+      <c r="AK114" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AL114" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AM114" s="26"/>
-      <c r="AN114" s="26"/>
+      <c r="AN114" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AO114" s="26"/>
-      <c r="AP114" s="26"/>
+      <c r="AP114" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AQ114" s="26"/>
       <c r="AR114" s="26"/>
       <c r="AS114" s="26"/>
@@ -10182,29 +10567,57 @@
     </row>
     <row r="115">
       <c r="A115" s="28"/>
-      <c r="B115" s="14"/>
-      <c r="C115" s="26"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="17"/>
-      <c r="F115" s="59"/>
+      <c r="B115" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C115" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D115" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E115" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F115" s="59" t="s">
+        <v>138</v>
+      </c>
       <c r="G115" s="21"/>
-      <c r="H115" s="21"/>
-      <c r="I115" s="26"/>
-      <c r="J115" s="26"/>
-      <c r="K115" s="63"/>
-      <c r="L115" s="26"/>
+      <c r="H115" s="21">
+        <v>320000.0</v>
+      </c>
+      <c r="I115" s="35"/>
+      <c r="J115" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="K115" s="21">
+        <v>20000.0</v>
+      </c>
+      <c r="L115" s="35">
+        <v>45.0</v>
+      </c>
       <c r="M115" s="26"/>
       <c r="N115" s="27"/>
-      <c r="O115" s="26"/>
+      <c r="O115" s="35" t="s">
+        <v>73</v>
+      </c>
       <c r="P115" s="26"/>
-      <c r="Q115" s="26"/>
-      <c r="R115" s="26"/>
+      <c r="Q115" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="R115" s="35">
+        <v>210.0</v>
+      </c>
       <c r="S115" s="26"/>
       <c r="T115" s="26"/>
       <c r="U115" s="64"/>
-      <c r="V115" s="55"/>
+      <c r="V115" s="61">
+        <v>1.0</v>
+      </c>
       <c r="W115" s="55"/>
-      <c r="X115" s="55"/>
+      <c r="X115" s="61">
+        <v>1.0</v>
+      </c>
       <c r="Y115" s="55"/>
       <c r="Z115" s="26"/>
       <c r="AA115" s="26"/>
@@ -10212,17 +10625,27 @@
       <c r="AC115" s="26"/>
       <c r="AD115" s="26"/>
       <c r="AE115" s="26"/>
-      <c r="AF115" s="26"/>
-      <c r="AG115" s="26"/>
-      <c r="AH115" s="26"/>
-      <c r="AI115" s="26"/>
+      <c r="AF115" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG115" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH115" s="35"/>
+      <c r="AI115" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AJ115" s="26"/>
-      <c r="AK115" s="26"/>
+      <c r="AK115" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AL115" s="26"/>
       <c r="AM115" s="26"/>
       <c r="AN115" s="26"/>
       <c r="AO115" s="26"/>
-      <c r="AP115" s="26"/>
+      <c r="AP115" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AQ115" s="26"/>
       <c r="AR115" s="26"/>
       <c r="AS115" s="26"/>
@@ -10240,9 +10663,15 @@
     </row>
     <row r="116">
       <c r="A116" s="28"/>
-      <c r="B116" s="14"/>
-      <c r="C116" s="26"/>
-      <c r="D116" s="17"/>
+      <c r="B116" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C116" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="D116" s="17" t="s">
+        <v>225</v>
+      </c>
       <c r="E116" s="17"/>
       <c r="F116" s="59"/>
       <c r="G116" s="21"/>
@@ -67139,10 +67568,10 @@
   </sheetData>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C76 C78:C1096">
-      <formula1>Types!$A$3:$A$8</formula1>
+      <formula1>Types!$A$3:$A$9</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D1:D200">
-      <formula1>Types!$C$3:$C$6</formula1>
+      <formula1>Types!$C$3:$C$8</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -67208,22 +67637,22 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="67" t="s">
-        <v>243</v>
+        <v>267</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="D2" s="67" t="s">
-        <v>246</v>
+        <v>270</v>
       </c>
       <c r="E2" s="67" t="s">
         <v>134</v>
       </c>
       <c r="F2" s="66" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
     </row>
     <row r="3">
@@ -67245,11 +67674,11 @@
         <v>44.0</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
       <c r="C4" s="22"/>
       <c r="E4" s="68" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5">
@@ -67257,11 +67686,11 @@
         <v>44.0</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="C5" s="22"/>
       <c r="E5" s="68" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6">
@@ -67269,11 +67698,11 @@
         <v>44.0</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
       <c r="C6" s="22"/>
       <c r="E6" s="68" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7">
@@ -67281,10 +67710,10 @@
         <v>62.0</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="E7" s="68" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11">
@@ -67297,19 +67726,19 @@
     </row>
     <row r="12">
       <c r="A12" s="66" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="C12" s="66">
         <v>1000.0</v>
       </c>
       <c r="E12" s="68" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="F12" s="47" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
       <c r="G12" s="66" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -67340,10 +67769,10 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="69" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="C2" s="69" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3">
@@ -67359,7 +67788,7 @@
         <v>57</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5">
@@ -67367,25 +67796,36 @@
         <v>82</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="66" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>262</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="66" t="s">
-        <v>263</v>
+        <v>286</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="66" t="s">
-        <v>264</v>
+        <v>288</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="66" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rebuild with diff tsconfig
</commit_message>
<xml_diff>
--- a/src/integrator/files/kondos.xlsx
+++ b/src/integrator/files/kondos.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="301">
   <si>
     <t>slug</t>
   </si>
@@ -911,6 +911,53 @@
     <t>Loteamento</t>
   </si>
   <si>
+    <t>Green Village</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O Green Village é um condomínio com recursos básicos de lazer, mas bom contato com a natureza.
+Os lotes são a partir de 500m², custando a partir dos R$ 262 mil, podendo ser financiados em até 144x com sinal de 10%
+</t>
+  </si>
+  <si>
+    <t>mira incorporações</t>
+  </si>
+  <si>
+    <t>Ponte Nova</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Ponte Nova é um loteamento novo na região da Serra do Elefante, próximo de Mateus Leme, que fica a 50 mins de BH.
+	O loteamento está sem seu estado bruto, rodeado da natureza, mas já conta com energia, água, iluminação, e uma pavimentação de ruas, sem asfalto ainda.
+	Bom investimento para quem gosta de pegar a oportunidade bem no início.</t>
+  </si>
+  <si>
+    <t>hipro</t>
+  </si>
+  <si>
+    <t>35670-000</t>
+  </si>
+  <si>
+    <t>Alta Vista</t>
+  </si>
+  <si>
+    <t>text-ready</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	O Alta Vista é um condomínio simples de casas pré-planejadas, que fica a 1,4 km da lagoa de Lagoa Santa.
+	Enquanto as casas são novas, de 1 pavimento, com fiação elétrica subterrânea e aquecimento solar, o condomínio conta com  infraestrutura básica, além de um playground para as crianças.</t>
+  </si>
+  <si>
+    <t>Benza</t>
+  </si>
+  <si>
+    <t>Benza está sendo construído como um condomínio alto padrão, localizado na cidade histórica de São joão del Rei, em frente ao trevo da charmosa Tiradentes.
+Com lotes a partir de 448m² com vista direta para a serra de São José, ele se coloca como um bom investimento para quem deseja o sossego do interior aliado aos eventos e gastronomia de Tiradentes.
+O condomínio ficará pronto em dezembro de 2025, até lá as obras estão avançadas.
+Com um total de 326 lotes, todos com vista para a Serra de São José.</t>
+  </si>
+  <si>
+    <t>São João del Rey</t>
+  </si>
+  <si>
     <t>IDKONDO</t>
   </si>
   <si>
@@ -960,9 +1007,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>text-ready</t>
   </si>
   <si>
     <t>Prédios</t>
@@ -10727,54 +10771,116 @@
     </row>
     <row r="117">
       <c r="A117" s="28"/>
-      <c r="B117" s="14"/>
-      <c r="C117" s="26"/>
-      <c r="D117" s="17"/>
-      <c r="E117" s="17"/>
+      <c r="B117" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="C117" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D117" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E117" s="17" t="s">
+        <v>268</v>
+      </c>
       <c r="F117" s="59"/>
-      <c r="G117" s="21"/>
-      <c r="H117" s="21"/>
-      <c r="I117" s="26"/>
-      <c r="J117" s="26"/>
-      <c r="K117" s="63"/>
-      <c r="L117" s="26"/>
+      <c r="G117" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="H117" s="21">
+        <v>270000.0</v>
+      </c>
+      <c r="I117" s="35">
+        <v>700.0</v>
+      </c>
+      <c r="J117" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="K117" s="21">
+        <v>500.0</v>
+      </c>
+      <c r="L117" s="35">
+        <v>40.0</v>
+      </c>
       <c r="M117" s="26"/>
       <c r="N117" s="27"/>
-      <c r="O117" s="26"/>
+      <c r="O117" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="P117" s="26"/>
-      <c r="Q117" s="26"/>
-      <c r="R117" s="26"/>
+      <c r="Q117" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="R117" s="35">
+        <v>144.0</v>
+      </c>
       <c r="S117" s="26"/>
-      <c r="T117" s="26"/>
+      <c r="T117" s="35">
+        <v>10.0</v>
+      </c>
       <c r="U117" s="64"/>
-      <c r="V117" s="55"/>
-      <c r="W117" s="55"/>
-      <c r="X117" s="55"/>
-      <c r="Y117" s="55"/>
-      <c r="Z117" s="26"/>
+      <c r="V117" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="W117" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="X117" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="Y117" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="Z117" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AA117" s="26"/>
-      <c r="AB117" s="26"/>
+      <c r="AB117" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AC117" s="26"/>
-      <c r="AD117" s="26"/>
+      <c r="AD117" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AE117" s="26"/>
-      <c r="AF117" s="26"/>
-      <c r="AG117" s="26"/>
-      <c r="AH117" s="26"/>
+      <c r="AF117" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG117" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH117" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AI117" s="26"/>
       <c r="AJ117" s="26"/>
-      <c r="AK117" s="26"/>
-      <c r="AL117" s="26"/>
+      <c r="AK117" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AL117" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AM117" s="26"/>
-      <c r="AN117" s="26"/>
+      <c r="AN117" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AO117" s="26"/>
-      <c r="AP117" s="26"/>
-      <c r="AQ117" s="26"/>
+      <c r="AP117" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AQ117" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AR117" s="26"/>
       <c r="AS117" s="26"/>
       <c r="AT117" s="26"/>
       <c r="AU117" s="26"/>
-      <c r="AV117" s="26"/>
-      <c r="AW117" s="26"/>
+      <c r="AV117" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AW117" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AX117" s="26"/>
       <c r="AY117" s="26"/>
       <c r="AZ117" s="27"/>
@@ -10785,23 +10891,53 @@
     </row>
     <row r="118">
       <c r="A118" s="28"/>
-      <c r="B118" s="14"/>
-      <c r="C118" s="26"/>
-      <c r="D118" s="17"/>
-      <c r="E118" s="17"/>
-      <c r="F118" s="59"/>
-      <c r="G118" s="21"/>
-      <c r="H118" s="21"/>
-      <c r="I118" s="26"/>
-      <c r="J118" s="26"/>
-      <c r="K118" s="63"/>
-      <c r="L118" s="26"/>
-      <c r="M118" s="26"/>
+      <c r="B118" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="C118" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D118" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E118" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="F118" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="G118" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="H118" s="21">
+        <v>75000.0</v>
+      </c>
+      <c r="I118" s="35">
+        <v>0.0</v>
+      </c>
+      <c r="J118" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="K118" s="21">
+        <v>1000.0</v>
+      </c>
+      <c r="L118" s="35">
+        <v>55.0</v>
+      </c>
+      <c r="M118" s="35" t="s">
+        <v>273</v>
+      </c>
       <c r="N118" s="27"/>
-      <c r="O118" s="26"/>
+      <c r="O118" s="35" t="s">
+        <v>94</v>
+      </c>
       <c r="P118" s="26"/>
-      <c r="Q118" s="26"/>
-      <c r="R118" s="26"/>
+      <c r="Q118" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="R118" s="35">
+        <v>96.0</v>
+      </c>
       <c r="S118" s="26"/>
       <c r="T118" s="26"/>
       <c r="U118" s="64"/>
@@ -10815,15 +10951,25 @@
       <c r="AC118" s="26"/>
       <c r="AD118" s="26"/>
       <c r="AE118" s="26"/>
-      <c r="AF118" s="26"/>
-      <c r="AG118" s="26"/>
+      <c r="AF118" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG118" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AH118" s="26"/>
       <c r="AI118" s="26"/>
       <c r="AJ118" s="26"/>
-      <c r="AK118" s="26"/>
-      <c r="AL118" s="26"/>
+      <c r="AK118" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AL118" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AM118" s="26"/>
-      <c r="AN118" s="26"/>
+      <c r="AN118" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AO118" s="26"/>
       <c r="AP118" s="26"/>
       <c r="AQ118" s="26"/>
@@ -10843,14 +10989,24 @@
     </row>
     <row r="119">
       <c r="A119" s="28"/>
-      <c r="B119" s="14"/>
-      <c r="C119" s="26"/>
-      <c r="D119" s="17"/>
-      <c r="E119" s="17"/>
+      <c r="B119" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="C119" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D119" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="E119" s="17" t="s">
+        <v>276</v>
+      </c>
       <c r="F119" s="59"/>
       <c r="G119" s="21"/>
       <c r="H119" s="21"/>
-      <c r="I119" s="26"/>
+      <c r="I119" s="35">
+        <v>500.0</v>
+      </c>
       <c r="J119" s="26"/>
       <c r="K119" s="63"/>
       <c r="L119" s="26"/>
@@ -10901,39 +11057,77 @@
     </row>
     <row r="120">
       <c r="A120" s="28"/>
-      <c r="B120" s="14"/>
-      <c r="C120" s="26"/>
-      <c r="D120" s="17"/>
-      <c r="E120" s="17"/>
-      <c r="F120" s="59"/>
+      <c r="B120" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C120" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D120" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E120" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="F120" s="59" t="s">
+        <v>138</v>
+      </c>
       <c r="G120" s="21"/>
       <c r="H120" s="21"/>
       <c r="I120" s="26"/>
-      <c r="J120" s="26"/>
-      <c r="K120" s="63"/>
-      <c r="L120" s="26"/>
+      <c r="J120" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="K120" s="21">
+        <v>450.0</v>
+      </c>
+      <c r="L120" s="35">
+        <v>180.0</v>
+      </c>
       <c r="M120" s="26"/>
       <c r="N120" s="27"/>
-      <c r="O120" s="26"/>
+      <c r="O120" s="35" t="s">
+        <v>279</v>
+      </c>
       <c r="P120" s="26"/>
       <c r="Q120" s="26"/>
       <c r="R120" s="26"/>
       <c r="S120" s="26"/>
       <c r="T120" s="26"/>
       <c r="U120" s="64"/>
-      <c r="V120" s="55"/>
-      <c r="W120" s="55"/>
-      <c r="X120" s="55"/>
+      <c r="V120" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="W120" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="X120" s="61">
+        <v>1.0</v>
+      </c>
       <c r="Y120" s="55"/>
-      <c r="Z120" s="26"/>
-      <c r="AA120" s="26"/>
-      <c r="AB120" s="26"/>
+      <c r="Z120" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AA120" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AB120" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AC120" s="26"/>
-      <c r="AD120" s="26"/>
+      <c r="AD120" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AE120" s="26"/>
-      <c r="AF120" s="26"/>
-      <c r="AG120" s="26"/>
-      <c r="AH120" s="26"/>
+      <c r="AF120" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG120" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH120" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AI120" s="26"/>
       <c r="AJ120" s="26"/>
       <c r="AK120" s="26"/>
@@ -10945,11 +11139,19 @@
       <c r="AQ120" s="26"/>
       <c r="AR120" s="26"/>
       <c r="AS120" s="26"/>
-      <c r="AT120" s="26"/>
+      <c r="AT120" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AU120" s="26"/>
-      <c r="AV120" s="26"/>
-      <c r="AW120" s="26"/>
-      <c r="AX120" s="26"/>
+      <c r="AV120" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AW120" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AX120" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AY120" s="26"/>
       <c r="AZ120" s="27"/>
       <c r="BA120" s="27"/>
@@ -67637,22 +67839,22 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="67" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="D2" s="67" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="E2" s="67" t="s">
         <v>134</v>
       </c>
       <c r="F2" s="66" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3">
@@ -67674,11 +67876,11 @@
         <v>44.0</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="C4" s="22"/>
       <c r="E4" s="68" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5">
@@ -67686,11 +67888,11 @@
         <v>44.0</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>274</v>
+        <v>287</v>
       </c>
       <c r="C5" s="22"/>
       <c r="E5" s="68" t="s">
-        <v>275</v>
+        <v>288</v>
       </c>
     </row>
     <row r="6">
@@ -67698,11 +67900,11 @@
         <v>44.0</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>276</v>
+        <v>289</v>
       </c>
       <c r="C6" s="22"/>
       <c r="E6" s="68" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7">
@@ -67710,10 +67912,10 @@
         <v>62.0</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>278</v>
+        <v>291</v>
       </c>
       <c r="E7" s="68" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11">
@@ -67726,19 +67928,19 @@
     </row>
     <row r="12">
       <c r="A12" s="66" t="s">
-        <v>280</v>
+        <v>293</v>
       </c>
       <c r="C12" s="66">
         <v>1000.0</v>
       </c>
       <c r="E12" s="68" t="s">
-        <v>273</v>
+        <v>286</v>
       </c>
       <c r="F12" s="47" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="G12" s="66" t="s">
-        <v>281</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -67769,10 +67971,10 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="69" t="s">
-        <v>282</v>
+        <v>295</v>
       </c>
       <c r="C2" s="69" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3">
@@ -67788,7 +67990,7 @@
         <v>57</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5">
@@ -67801,7 +68003,7 @@
     </row>
     <row r="6">
       <c r="A6" s="66" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="C6" s="66" t="s">
         <v>211</v>
@@ -67809,15 +68011,15 @@
     </row>
     <row r="7">
       <c r="A7" s="66" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="66" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="C8" s="66" t="s">
         <v>225</v>

</xml_diff>

<commit_message>
now getting only DONE kondos
</commit_message>
<xml_diff>
--- a/src/integrator/files/kondos.xlsx
+++ b/src/integrator/files/kondos.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="314">
   <si>
     <t>slug</t>
   </si>
@@ -958,6 +958,53 @@
     <t>São João del Rey</t>
   </si>
   <si>
+    <t>Sensia pampulha</t>
+  </si>
+  <si>
+    <t>Prédios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Sensia é um super condomínio de 3 prédios, localizado na região da pampulha, com todos os recursos de um clube.
+	Os apartamentos são personalizáveis de 62m² a 80m², podendo ser 2 ou 3 quartos com suíte e varanda gourmet.
+	A área de lazer e recursos do condomínio impressionam, com piscinas, sauna, espaço de massagem, espaço kids, academia, área gourmet e muito mais.
+	Fica muito bem localizado no bairro Liberdade, próximo da lagoa da pampulha.</t>
+  </si>
+  <si>
+    <t>mrv</t>
+  </si>
+  <si>
+    <t>Rua General Aranha, 340</t>
+  </si>
+  <si>
+    <t>Belo Horizonte</t>
+  </si>
+  <si>
+    <t>Liberdade</t>
+  </si>
+  <si>
+    <t>Jardim Linhares</t>
+  </si>
+  <si>
+    <t>Retiro das Aguas</t>
+  </si>
+  <si>
+    <t>Lumina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Com apartamentos de 3 quartos com suíte, o Lúmina é um condomínio que impõe respeito. 
+Possui uma área de lazer bem gourmet, com piscina, academia, área kids, e um espaço de convivencia gourmet bem agradável.
+</t>
+  </si>
+  <si>
+    <t>CMC Castro</t>
+  </si>
+  <si>
+    <t>Rua Clóvis Magalhães Pinto, 214</t>
+  </si>
+  <si>
+    <t>Cidade Nova</t>
+  </si>
+  <si>
     <t>IDKONDO</t>
   </si>
   <si>
@@ -1007,9 +1054,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Prédios</t>
   </si>
   <si>
     <t>Comercial</t>
@@ -1768,7 +1812,7 @@
     <col customWidth="1" min="18" max="18" width="16.13"/>
     <col customWidth="1" min="19" max="19" width="12.13"/>
     <col customWidth="1" min="20" max="20" width="18.5"/>
-    <col customWidth="1" min="21" max="21" width="58.75"/>
+    <col customWidth="1" min="21" max="21" width="44.13"/>
     <col customWidth="1" min="22" max="22" width="15.0"/>
     <col customWidth="1" min="23" max="23" width="13.0"/>
     <col customWidth="1" min="24" max="24" width="9.5"/>
@@ -11161,55 +11205,123 @@
     </row>
     <row r="121">
       <c r="A121" s="28"/>
-      <c r="B121" s="14"/>
-      <c r="C121" s="26"/>
-      <c r="D121" s="17"/>
-      <c r="E121" s="17"/>
-      <c r="F121" s="59"/>
-      <c r="G121" s="21"/>
+      <c r="B121" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C121" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="D121" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E121" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="F121" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="G121" s="21" t="s">
+        <v>283</v>
+      </c>
       <c r="H121" s="21"/>
-      <c r="I121" s="26"/>
+      <c r="I121" s="35">
+        <v>700.0</v>
+      </c>
       <c r="J121" s="26"/>
       <c r="K121" s="63"/>
-      <c r="L121" s="26"/>
+      <c r="L121" s="35">
+        <v>0.0</v>
+      </c>
       <c r="M121" s="26"/>
-      <c r="N121" s="27"/>
-      <c r="O121" s="26"/>
-      <c r="P121" s="26"/>
-      <c r="Q121" s="26"/>
+      <c r="N121" s="42" t="s">
+        <v>284</v>
+      </c>
+      <c r="O121" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="P121" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q121" s="35">
+        <v>1.0</v>
+      </c>
       <c r="R121" s="26"/>
       <c r="S121" s="26"/>
       <c r="T121" s="26"/>
       <c r="U121" s="64"/>
-      <c r="V121" s="55"/>
-      <c r="W121" s="55"/>
-      <c r="X121" s="55"/>
-      <c r="Y121" s="55"/>
-      <c r="Z121" s="26"/>
-      <c r="AA121" s="26"/>
-      <c r="AB121" s="26"/>
-      <c r="AC121" s="26"/>
-      <c r="AD121" s="26"/>
-      <c r="AE121" s="26"/>
-      <c r="AF121" s="26"/>
-      <c r="AG121" s="26"/>
-      <c r="AH121" s="26"/>
-      <c r="AI121" s="26"/>
-      <c r="AJ121" s="26"/>
+      <c r="V121" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="W121" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="X121" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="Y121" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="Z121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AA121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AB121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AC121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AD121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AE121" s="35"/>
+      <c r="AF121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AI121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AJ121" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AK121" s="26"/>
       <c r="AL121" s="26"/>
       <c r="AM121" s="26"/>
       <c r="AN121" s="26"/>
-      <c r="AO121" s="26"/>
+      <c r="AO121" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AP121" s="26"/>
-      <c r="AQ121" s="26"/>
-      <c r="AR121" s="26"/>
+      <c r="AQ121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AR121" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AS121" s="26"/>
-      <c r="AT121" s="26"/>
-      <c r="AU121" s="26"/>
-      <c r="AV121" s="26"/>
-      <c r="AW121" s="26"/>
-      <c r="AX121" s="26"/>
+      <c r="AT121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AU121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AV121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AW121" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AX121" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AY121" s="26"/>
       <c r="AZ121" s="27"/>
       <c r="BA121" s="27"/>
@@ -11219,9 +11331,15 @@
     </row>
     <row r="122">
       <c r="A122" s="28"/>
-      <c r="B122" s="14"/>
-      <c r="C122" s="26"/>
-      <c r="D122" s="17"/>
+      <c r="B122" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C122" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="D122" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E122" s="17"/>
       <c r="F122" s="59"/>
       <c r="G122" s="21"/>
@@ -11277,9 +11395,15 @@
     </row>
     <row r="123">
       <c r="A123" s="28"/>
-      <c r="B123" s="14"/>
-      <c r="C123" s="26"/>
-      <c r="D123" s="17"/>
+      <c r="B123" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="C123" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D123" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="E123" s="17"/>
       <c r="F123" s="59"/>
       <c r="G123" s="21"/>
@@ -11335,40 +11459,82 @@
     </row>
     <row r="124">
       <c r="A124" s="28"/>
-      <c r="B124" s="14"/>
-      <c r="C124" s="26"/>
-      <c r="D124" s="17"/>
-      <c r="E124" s="17"/>
-      <c r="F124" s="59"/>
-      <c r="G124" s="21"/>
+      <c r="B124" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="C124" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="D124" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E124" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="F124" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="G124" s="21" t="s">
+        <v>291</v>
+      </c>
       <c r="H124" s="21"/>
-      <c r="I124" s="26"/>
+      <c r="I124" s="35">
+        <v>500.0</v>
+      </c>
       <c r="J124" s="26"/>
       <c r="K124" s="63"/>
-      <c r="L124" s="26"/>
+      <c r="L124" s="35">
+        <v>0.0</v>
+      </c>
       <c r="M124" s="26"/>
-      <c r="N124" s="27"/>
+      <c r="N124" s="42" t="s">
+        <v>292</v>
+      </c>
       <c r="O124" s="26"/>
-      <c r="P124" s="26"/>
+      <c r="P124" s="35" t="s">
+        <v>293</v>
+      </c>
       <c r="Q124" s="26"/>
       <c r="R124" s="26"/>
       <c r="S124" s="26"/>
       <c r="T124" s="26"/>
       <c r="U124" s="64"/>
-      <c r="V124" s="55"/>
-      <c r="W124" s="55"/>
-      <c r="X124" s="55"/>
+      <c r="V124" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="W124" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="X124" s="61">
+        <v>1.0</v>
+      </c>
       <c r="Y124" s="55"/>
-      <c r="Z124" s="26"/>
-      <c r="AA124" s="26"/>
-      <c r="AB124" s="26"/>
+      <c r="Z124" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AA124" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AB124" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AC124" s="26"/>
-      <c r="AD124" s="26"/>
+      <c r="AD124" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AE124" s="26"/>
-      <c r="AF124" s="26"/>
-      <c r="AG124" s="26"/>
-      <c r="AH124" s="26"/>
-      <c r="AI124" s="26"/>
+      <c r="AF124" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AG124" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AH124" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AI124" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AJ124" s="26"/>
       <c r="AK124" s="26"/>
       <c r="AL124" s="26"/>
@@ -11376,14 +11542,22 @@
       <c r="AN124" s="26"/>
       <c r="AO124" s="26"/>
       <c r="AP124" s="26"/>
-      <c r="AQ124" s="26"/>
-      <c r="AR124" s="26"/>
+      <c r="AQ124" s="35">
+        <v>1.0</v>
+      </c>
+      <c r="AR124" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AS124" s="26"/>
-      <c r="AT124" s="26"/>
+      <c r="AT124" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AU124" s="26"/>
       <c r="AV124" s="26"/>
       <c r="AW124" s="26"/>
-      <c r="AX124" s="26"/>
+      <c r="AX124" s="35">
+        <v>1.0</v>
+      </c>
       <c r="AY124" s="26"/>
       <c r="AZ124" s="27"/>
       <c r="BA124" s="27"/>
@@ -67839,22 +68013,22 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="67" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="D2" s="67" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="E2" s="67" t="s">
         <v>134</v>
       </c>
       <c r="F2" s="66" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3">
@@ -67876,11 +68050,11 @@
         <v>44.0</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="C4" s="22"/>
       <c r="E4" s="68" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5">
@@ -67888,11 +68062,11 @@
         <v>44.0</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C5" s="22"/>
       <c r="E5" s="68" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6">
@@ -67900,11 +68074,11 @@
         <v>44.0</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="C6" s="22"/>
       <c r="E6" s="68" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
     </row>
     <row r="7">
@@ -67912,10 +68086,10 @@
         <v>62.0</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="E7" s="68" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11">
@@ -67928,19 +68102,19 @@
     </row>
     <row r="12">
       <c r="A12" s="66" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="C12" s="66">
         <v>1000.0</v>
       </c>
       <c r="E12" s="68" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="F12" s="47" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="G12" s="66" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -67971,10 +68145,10 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="69" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="C2" s="69" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3">
@@ -68003,7 +68177,7 @@
     </row>
     <row r="6">
       <c r="A6" s="66" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="C6" s="66" t="s">
         <v>211</v>
@@ -68011,15 +68185,15 @@
     </row>
     <row r="7">
       <c r="A7" s="66" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="66" t="s">
-        <v>300</v>
+        <v>313</v>
       </c>
       <c r="C8" s="66" t="s">
         <v>225</v>

</xml_diff>